<commit_message>
Added more use cases to Project Charter.xls
</commit_message>
<xml_diff>
--- a/docs/Project Charter.xlsx
+++ b/docs/Project Charter.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afrol\OneDrive\Documents\Capstone\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afrol\OneDrive\Documents\Capstone\GitHub\easysched\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="11_F25DC773A252ABDACC1048D9619E7A2A5ADE58E9" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{28F1E113-C809-495B-B180-A02D9BBF71BF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44DAEADB-4415-485F-B4C1-163F2DCD07C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="69">
   <si>
     <t>Event</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Employer wants to delete a schedule</t>
   </si>
   <si>
-    <t xml:space="preserve">Employer wants to </t>
-  </si>
-  <si>
     <t xml:space="preserve">Employer wants to view a schedule </t>
   </si>
   <si>
@@ -67,16 +64,190 @@
   </si>
   <si>
     <t>Employer wants to create an employee in the system</t>
+  </si>
+  <si>
+    <t>Employer wants to view employees</t>
+  </si>
+  <si>
+    <t>Employer wants to delete an employee from the system</t>
+  </si>
+  <si>
+    <t>Employer wants to display a message to the employees</t>
+  </si>
+  <si>
+    <t>Employee wants to view a schedule</t>
+  </si>
+  <si>
+    <t>Employee wants to update their availability</t>
+  </si>
+  <si>
+    <t>Employee wants to request time off</t>
+  </si>
+  <si>
+    <t>Employee wants to give another employee a shift</t>
+  </si>
+  <si>
+    <t>Employee wants to trade a shift with another employee</t>
+  </si>
+  <si>
+    <t>Employer</t>
+  </si>
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>UC01</t>
+  </si>
+  <si>
+    <t>UC02</t>
+  </si>
+  <si>
+    <t>UC03</t>
+  </si>
+  <si>
+    <t>UC04</t>
+  </si>
+  <si>
+    <t>UC05</t>
+  </si>
+  <si>
+    <t>UC06</t>
+  </si>
+  <si>
+    <t>UC07</t>
+  </si>
+  <si>
+    <t>UC08</t>
+  </si>
+  <si>
+    <t>UC09</t>
+  </si>
+  <si>
+    <t>UC10</t>
+  </si>
+  <si>
+    <t>UC11</t>
+  </si>
+  <si>
+    <t>UC12</t>
+  </si>
+  <si>
+    <t>UC13</t>
+  </si>
+  <si>
+    <t>UC14</t>
+  </si>
+  <si>
+    <t>Create Schedule</t>
+  </si>
+  <si>
+    <t>Edit Schedule</t>
+  </si>
+  <si>
+    <t>Delete Schedule</t>
+  </si>
+  <si>
+    <t>Update Availability</t>
+  </si>
+  <si>
+    <t>Admin View Schedule</t>
+  </si>
+  <si>
+    <t>Admin Edit Employee Information</t>
+  </si>
+  <si>
+    <t>Create Employee</t>
+  </si>
+  <si>
+    <t>View Employees</t>
+  </si>
+  <si>
+    <t>Delete Employee</t>
+  </si>
+  <si>
+    <t>Message Employees</t>
+  </si>
+  <si>
+    <t>Employee View Schedule</t>
+  </si>
+  <si>
+    <t>Employee wants to edit their personal information</t>
+  </si>
+  <si>
+    <t>UC15</t>
+  </si>
+  <si>
+    <t>Request Time Off</t>
+  </si>
+  <si>
+    <t>Employee Give Shift</t>
+  </si>
+  <si>
+    <t>Employee Trade Shift</t>
+  </si>
+  <si>
+    <t>Employee Edit Information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A schedule is created </t>
+  </si>
+  <si>
+    <t>A change is made to an existing schedule</t>
+  </si>
+  <si>
+    <t>A schedule is deleted</t>
+  </si>
+  <si>
+    <t>A list of schedules is displayed</t>
+  </si>
+  <si>
+    <t>Existing employee information is changed</t>
+  </si>
+  <si>
+    <t>An employee is added into the system</t>
+  </si>
+  <si>
+    <t>A list of employees is displayed</t>
+  </si>
+  <si>
+    <t>An employees information is removed form the system</t>
+  </si>
+  <si>
+    <t>A message is displayed to users of the system</t>
+  </si>
+  <si>
+    <t>A schedule is displayed</t>
+  </si>
+  <si>
+    <t>Availability is updated</t>
+  </si>
+  <si>
+    <t>A request is submitted to the employer of when desired time is to be booked off</t>
+  </si>
+  <si>
+    <t>A request is submitted to the employer of who will be taking a particular shift</t>
+  </si>
+  <si>
+    <t>A request is submitted to the employer of who will be taking which shifts</t>
+  </si>
+  <si>
+    <t>A change is made to the employees information</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -387,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -399,8 +570,8 @@
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -417,10 +588,10 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G1" t="s">
@@ -431,38 +602,259 @@
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>12</v>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>